<commit_message>
Added run_all bash file
</commit_message>
<xml_diff>
--- a/models/dft/dcas/properties.xlsx
+++ b/models/dft/dcas/properties.xlsx
@@ -4,11 +4,10 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
-    <sheet name="Properties_more" sheetId="3" r:id="rId1"/>
-    <sheet name="Properties" sheetId="2" r:id="rId2"/>
+    <sheet name="Properties" sheetId="3" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t>failed</t>
   </si>
@@ -340,10 +339,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A31"/>
+  <dimension ref="A1:A26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -355,181 +354,151 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>1000</v>
+        <f>16000*1/25</f>
+        <v>640</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>2000</v>
+        <f>A2+$A$2</f>
+        <v>1280</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>3000</v>
+        <f t="shared" ref="A4:A25" si="0">A3+$A$2</f>
+        <v>1920</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>4000</v>
+        <f t="shared" si="0"/>
+        <v>2560</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>5000</v>
+        <f t="shared" si="0"/>
+        <v>3200</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>6000</v>
+        <f t="shared" si="0"/>
+        <v>3840</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>7000</v>
+        <f t="shared" si="0"/>
+        <v>4480</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>8000</v>
+        <f t="shared" si="0"/>
+        <v>5120</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>9000</v>
+        <f t="shared" si="0"/>
+        <v>5760</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>10000</v>
+        <f t="shared" si="0"/>
+        <v>6400</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>11000</v>
+        <f t="shared" si="0"/>
+        <v>7040</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>12000</v>
+        <f t="shared" si="0"/>
+        <v>7680</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>13000</v>
+        <f t="shared" si="0"/>
+        <v>8320</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>14000</v>
+        <f t="shared" si="0"/>
+        <v>8960</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>15000</v>
+        <f t="shared" si="0"/>
+        <v>9600</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>16000</v>
+        <f t="shared" si="0"/>
+        <v>10240</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>17000</v>
+        <f t="shared" si="0"/>
+        <v>10880</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>18000</v>
+        <f t="shared" si="0"/>
+        <v>11520</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>19000</v>
+        <f t="shared" si="0"/>
+        <v>12160</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>20000</v>
+        <f t="shared" si="0"/>
+        <v>12800</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>21000</v>
+        <f t="shared" si="0"/>
+        <v>13440</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>22000</v>
+        <f t="shared" si="0"/>
+        <v>14080</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>23000</v>
+        <f t="shared" si="0"/>
+        <v>14720</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25">
-        <v>24000</v>
+        <f t="shared" si="0"/>
+        <v>15360</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26">
-        <v>25000</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27">
-        <v>26000</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A28">
-        <v>27000</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A29">
-        <v>28000</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A30">
-        <v>29000</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A31">
-        <v>30000</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F60" sqref="F60"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>6000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3">
+        <f t="shared" ref="A4:A36" si="1">A25+$A$2</f>
         <v>16000</v>
       </c>
     </row>

</xml_diff>